<commit_message>
Malayalam entry fix and file upload strategy
</commit_message>
<xml_diff>
--- a/output/student_ids.xlsx
+++ b/output/student_ids.xlsx
@@ -412,7 +412,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>680f69dda7775d4878a8370d</v>
+        <v>6810692cdc110c0f6972b99c</v>
       </c>
       <c r="B2" t="str">
         <v>REUBEN REPSOL</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>680f69dda7775d4878a83735</v>
+        <v>6810692cdc110c0f6972b9c4</v>
       </c>
       <c r="B3" t="str">
         <v>JOHAN JESWIN</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>680f69dda7775d4878a8375d</v>
+        <v>6810692cdc110c0f6972b9ec</v>
       </c>
       <c r="B4" t="str">
         <v>ARUN K B</v>

</xml_diff>